<commit_message>
add documents, fix admin/book
</commit_message>
<xml_diff>
--- a/document/Client_Testcase.xlsx
+++ b/document/Client_Testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Project\HCL\Book-Final\final\bookstore\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B65F45-7DAB-4C1B-9610-393BF03FE367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFDBD8C-F73B-4C1A-B1F3-83621E410B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9ECE07E4-03FA-4E68-B4DD-19ECE20BFDB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9ECE07E4-03FA-4E68-B4DD-19ECE20BFDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Login&amp;Registration" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="214">
   <si>
     <t>Test  Cases  Report</t>
   </si>
@@ -792,6 +792,142 @@
   </si>
   <si>
     <t>Card is deleted in database</t>
+  </si>
+  <si>
+    <t>UserName: tungnt
+Password: 12345678</t>
+  </si>
+  <si>
+    <t>UserName: 
+Password: Abcd1234.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tung
+Password: </t>
+  </si>
+  <si>
+    <t>Username: tung123
+Password: Abcd1234.</t>
+  </si>
+  <si>
+    <t>Username: tung123
+Password: Abcd123123123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: Abcd1234.
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName:
+Password: Abcd1234.
+RePassword: Abcd1234.
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password:
+RePassword: 
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: abcd1234654
+RePassword: abcd1234654
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: 
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: Abcd123445.
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: Abcd1234.
+Name: Tung Nguyen
+Email: 
+Dob: 04/11/2000
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: Abcd1234.
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 
+Phone: 09611111111
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName: tungnt1234
+Password: Abcd1234.
+RePassword: Abcd1234.
+Name: Tung Nguyen
+Email: tungnt@gmail.com
+Dob: 04/11/2000
+Phone: 
+</t>
+  </si>
+  <si>
+    <t>input existing UserName</t>
+  </si>
+  <si>
+    <t>Existing UserName: tungnt
+Input UserName: tungnt</t>
+  </si>
+  <si>
+    <t>An error message "Account Exists"</t>
+  </si>
+  <si>
+    <t>UserName must be unique</t>
+  </si>
+  <si>
+    <t>Email must be unique</t>
+  </si>
+  <si>
+    <t>input existing email</t>
+  </si>
+  <si>
+    <t>Existing UserName: natsu1504@gmail.com
+Input UserName: natsu1504@gmail.com</t>
+  </si>
+  <si>
+    <t>An error message "Email Exists"</t>
   </si>
 </sst>
 </file>
@@ -907,7 +1043,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -957,17 +1093,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -980,6 +1113,18 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1296,527 +1441,622 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B21FDF5-8BBD-486B-8E08-04C0D8F9DB9F}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.44140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="18" style="18" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="33.44140625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="10"/>
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="11" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="J2" s="19"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="11" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:10" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="J5" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="18">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="18">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="18">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="J9" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12" t="s">
+      <c r="G10" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="J10" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="J11" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="5" t="s">
+      <c r="G12" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="J12" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="J13" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
         <v>10</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="J14" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
         <v>11</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12" t="s">
+      <c r="G15" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="J15" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
         <v>12</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12" t="s">
+      <c r="G16" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="J16" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12" t="s">
+      <c r="G17" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="J17" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
         <v>14</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12" t="s">
+      <c r="G18" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>15</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>16</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1836,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4621482C-2DA9-433F-8176-37F108CF60AA}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1856,57 +2096,57 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="23"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -2988,57 +3228,57 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A1" s="10"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="19"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">

</xml_diff>